<commit_message>
Feat : Export Nilai
</commit_message>
<xml_diff>
--- a/public/template/Template_import_nilai.xlsx
+++ b/public/template/Template_import_nilai.xlsx
@@ -78,8 +78,24 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
+  <fonts count="23">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -569,133 +585,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -703,13 +719,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1248,7 +1264,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>

</xml_diff>

<commit_message>
Fix : Import Nilai and Aktifitas
</commit_message>
<xml_diff>
--- a/public/template/Template_import_nilai.xlsx
+++ b/public/template/Template_import_nilai.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>NIM</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>han</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>fsda</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>sdewq</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1276,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C10" sqref="C10:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.4285714285714" customWidth="1"/>
   </cols>
@@ -1417,6 +1432,151 @@
         <v>90</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3">
+        <v>9999999994</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>88</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3">
+        <v>9999999995</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>88</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>88</v>
+      </c>
+      <c r="I7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3">
+        <v>9999999996</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>90</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3">
+        <v>9999999997</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>88</v>
+      </c>
+      <c r="G9">
+        <v>88</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3">
+        <v>9999999998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+      <c r="G10">
+        <v>88</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Feat : calculate Bobot KHS
</commit_message>
<xml_diff>
--- a/public/template/Template_import_nilai.xlsx
+++ b/public/template/Template_import_nilai.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>NIM</t>
   </si>
@@ -82,6 +82,9 @@
   <si>
     <t>sdewq</t>
   </si>
+  <si>
+    <t>9999999910</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +96,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,9 +121,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -600,137 +615,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -740,8 +755,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1276,10 +1306,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:I10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1318,7 +1348,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3">
-        <v>9999999991</v>
+        <v>9999999999</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1346,8 +1376,8 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3">
-        <v>9999999992</v>
+      <c r="A3" s="4">
+        <v>9999999991</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1375,8 +1405,8 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="3">
-        <v>9999999993</v>
+      <c r="A4" s="5">
+        <v>9999999992</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1405,7 +1435,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3">
-        <v>9999999999</v>
+        <v>9999999993</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1433,7 +1463,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="3">
+      <c r="A6" s="6">
         <v>9999999994</v>
       </c>
       <c r="B6" t="s">
@@ -1462,7 +1492,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="3">
+      <c r="A7" s="6">
         <v>9999999995</v>
       </c>
       <c r="B7" t="s">
@@ -1491,7 +1521,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>9999999996</v>
       </c>
       <c r="B8" t="s">
@@ -1520,7 +1550,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>9999999997</v>
       </c>
       <c r="B9" t="s">
@@ -1549,7 +1579,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3">
+      <c r="A10" s="6">
         <v>9999999998</v>
       </c>
       <c r="B10" t="s">
@@ -1575,6 +1605,325 @@
       </c>
       <c r="I10">
         <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>88</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6">
+        <v>9999999911</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>88</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>90</v>
+      </c>
+      <c r="G12">
+        <v>88</v>
+      </c>
+      <c r="H12">
+        <v>88</v>
+      </c>
+      <c r="I12">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6">
+        <v>9999999912</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>90</v>
+      </c>
+      <c r="E13">
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>90</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="6">
+        <v>9999999913</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>88</v>
+      </c>
+      <c r="G14">
+        <v>88</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="6">
+        <v>9999999914</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>88</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="I15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="6">
+        <v>9999999915</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>88</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>90</v>
+      </c>
+      <c r="G16">
+        <v>88</v>
+      </c>
+      <c r="H16">
+        <v>88</v>
+      </c>
+      <c r="I16">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="6">
+        <v>9999999916</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <v>90</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>90</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="6">
+        <v>99999999917</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>88</v>
+      </c>
+      <c r="G18">
+        <v>88</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="6">
+        <v>9999999918</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>88</v>
+      </c>
+      <c r="G19">
+        <v>88</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="6">
+        <v>9999999919</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>88</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>50</v>
+      </c>
+      <c r="I20">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="8">
+        <v>9999999920</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>88</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>90</v>
+      </c>
+      <c r="G21">
+        <v>88</v>
+      </c>
+      <c r="H21">
+        <v>88</v>
+      </c>
+      <c r="I21">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>